<commit_message>
update gropin 3 variables
</commit_message>
<xml_diff>
--- a/gropin/schema/metadataschema1040.xlsx
+++ b/gropin/schema/metadataschema1040.xlsx
@@ -5247,6 +5247,11 @@
           <t>Vector[number]</t>
         </is>
       </c>
+      <c r="V133" t="inlineStr">
+        <is>
+          <t>seq(2.002,19.98001998002,length.out=10)</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5304,6 +5309,11 @@
           <t>Vector[number]</t>
         </is>
       </c>
+      <c r="V134" t="inlineStr">
+        <is>
+          <t>seq(4.004,7.49250749250749,length.out=10)</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5354,6 +5364,11 @@
       <c r="R135" t="inlineStr">
         <is>
           <t>Vector[number]</t>
+        </is>
+      </c>
+      <c r="V135" t="inlineStr">
+        <is>
+          <t>seq(0.95095,0.994005994005994,length.out=10)</t>
         </is>
       </c>
     </row>

</xml_diff>